<commit_message>
minor debug. Add DV
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/v19/hyperarc.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/v19/hyperarc.xlsx
@@ -2686,7 +2686,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,19 +2815,19 @@
       <c r="A9" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>158</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>